<commit_message>
Margin and caption updates
</commit_message>
<xml_diff>
--- a/Private_Insurance_Coverage_Datafile.xlsx
+++ b/Private_Insurance_Coverage_Datafile.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27815"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="200" yWindow="460" windowWidth="27620" windowHeight="13640"/>
+    <workbookView xWindow="640" yWindow="460" windowWidth="21840" windowHeight="14360"/>
   </bookViews>
   <sheets>
     <sheet name="DataViz-2015" sheetId="24" r:id="rId1"/>
@@ -302,24 +302,23 @@
     <t xml:space="preserve">DMHC </t>
   </si>
   <si>
-    <t>Health Net figures under DMHC include Health Net Community Solutions (note that commercial enrollment of HNCS is zero). Cigna figures under CDI include Connecticut General and Cigna Health and Life. For additional details see data file available as document download.</t>
+    <t>by Insurer, California, 2015</t>
   </si>
   <si>
-    <t>by Insurer, California, 2015</t>
+    <t xml:space="preserve">Health Net figures under DMHC include Health Net Community Solutions (note that commercial enrollment of HNCS is zero). Cigna figures under CDI include Connecticut General and Cigna Health and Life. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="33">
+  <numFmts count="34">
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.0"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
     <numFmt numFmtId="168" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="169" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="170" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
@@ -346,6 +345,8 @@
     <numFmt numFmtId="191" formatCode="&quot;3E13&quot;"/>
     <numFmt numFmtId="192" formatCode="&quot;$&quot;#,##0.0;[Red]\(&quot;$&quot;#,###.0\)"/>
     <numFmt numFmtId="193" formatCode="0.000000000"/>
+    <numFmt numFmtId="194" formatCode="&quot;$&quot;#,##0.00000"/>
+    <numFmt numFmtId="195" formatCode="&quot;$&quot;#,##0.0000000"/>
   </numFmts>
   <fonts count="114" x14ac:knownFonts="1">
     <font>
@@ -3880,7 +3881,7 @@
     <xf numFmtId="9" fontId="106" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="106" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -3991,7 +3992,6 @@
     <xf numFmtId="166" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="105" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -4007,12 +4007,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="16" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="113" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="112" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="112" fillId="2" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="105" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="194" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="195" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1822">
     <cellStyle name="_%(SignOnly)" xfId="10"/>
@@ -6140,43 +6144,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomRight" activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.6640625" customWidth="1"/>
     <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="42.1640625" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
     <col min="4" max="5" width="10.33203125" customWidth="1"/>
     <col min="6" max="6" width="10.5" customWidth="1"/>
     <col min="7" max="8" width="11.1640625" customWidth="1"/>
-    <col min="9" max="9" width="10.5" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
     <col min="10" max="10" width="22.83203125" customWidth="1"/>
     <col min="11" max="11" width="7.33203125" customWidth="1"/>
     <col min="12" max="12" width="10.1640625" customWidth="1"/>
+    <col min="13" max="13" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="78" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
       <c r="K2" s="38"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -6184,7 +6191,6 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -6203,7 +6209,7 @@
       <c r="B5" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="67" t="s">
+      <c r="C5" s="66" t="s">
         <v>43</v>
       </c>
       <c r="D5" s="54" t="s">
@@ -6244,22 +6250,22 @@
       <c r="D6" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="70">
+      <c r="E6" s="69">
         <v>656</v>
       </c>
       <c r="F6" s="58">
         <v>76332</v>
       </c>
-      <c r="G6" s="70">
+      <c r="G6" s="69">
         <v>152216</v>
       </c>
-      <c r="H6" s="70">
+      <c r="H6" s="69">
         <v>657248</v>
       </c>
       <c r="I6" s="64">
         <v>1.855697849</v>
       </c>
-      <c r="J6" s="75">
+      <c r="J6" s="74">
         <v>6.6274113603707274E-2</v>
       </c>
       <c r="K6" s="23">
@@ -6279,16 +6285,16 @@
       <c r="D7" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="71">
+      <c r="E7" s="70">
         <v>136092</v>
       </c>
       <c r="F7" s="59">
         <v>174</v>
       </c>
-      <c r="G7" s="71">
+      <c r="G7" s="70">
         <v>135830</v>
       </c>
-      <c r="H7" s="71">
+      <c r="H7" s="70">
         <v>2247449</v>
       </c>
       <c r="I7" s="65">
@@ -6314,16 +6320,16 @@
       <c r="D8" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="72">
+      <c r="E8" s="71">
         <v>44026</v>
       </c>
       <c r="F8" s="60">
         <v>0</v>
       </c>
-      <c r="G8" s="72">
+      <c r="G8" s="71">
         <v>10656</v>
       </c>
-      <c r="H8" s="72">
+      <c r="H8" s="71">
         <v>0</v>
       </c>
       <c r="I8" s="65">
@@ -6349,22 +6355,22 @@
       <c r="D9" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="72">
+      <c r="E9" s="71">
         <v>46931</v>
       </c>
       <c r="F9" s="60">
         <v>0</v>
       </c>
-      <c r="G9" s="72">
+      <c r="G9" s="71">
         <v>259164</v>
       </c>
-      <c r="H9" s="72">
+      <c r="H9" s="71">
         <v>1635310</v>
       </c>
       <c r="I9" s="65">
         <v>1.155211199</v>
       </c>
-      <c r="J9" s="82" t="s">
+      <c r="J9" s="79" t="s">
         <v>45</v>
       </c>
       <c r="K9" s="28">
@@ -6384,16 +6390,16 @@
       <c r="D10" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="71">
+      <c r="E10" s="70">
         <v>36330</v>
       </c>
       <c r="F10" s="59">
         <v>104885</v>
       </c>
-      <c r="G10" s="71">
+      <c r="G10" s="70">
         <v>20304</v>
       </c>
-      <c r="H10" s="71">
+      <c r="H10" s="70">
         <v>0</v>
       </c>
       <c r="I10" s="65">
@@ -6419,16 +6425,16 @@
       <c r="D11" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="71">
+      <c r="E11" s="70">
         <v>0</v>
       </c>
       <c r="F11" s="59">
         <v>1113</v>
       </c>
-      <c r="G11" s="71">
+      <c r="G11" s="70">
         <v>7404</v>
       </c>
-      <c r="H11" s="71">
+      <c r="H11" s="70">
         <v>140009</v>
       </c>
       <c r="I11" s="65">
@@ -6455,16 +6461,16 @@
       <c r="D12" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="71">
+      <c r="E12" s="70">
         <v>94</v>
       </c>
       <c r="F12" s="59">
         <v>44915</v>
       </c>
-      <c r="G12" s="71">
+      <c r="G12" s="70">
         <v>164823</v>
       </c>
-      <c r="H12" s="71">
+      <c r="H12" s="70">
         <v>807334</v>
       </c>
       <c r="I12" s="65">
@@ -6490,7 +6496,7 @@
       <c r="D13" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="73">
+      <c r="E13" s="72">
         <f>E25-SUM(E6:E12)</f>
         <v>56005</v>
       </c>
@@ -6498,11 +6504,11 @@
         <f>F25-SUM(F6:F12)</f>
         <v>18466</v>
       </c>
-      <c r="G13" s="73">
+      <c r="G13" s="72">
         <f>G25-SUM(G6:G12)</f>
         <v>56598</v>
       </c>
-      <c r="H13" s="73">
+      <c r="H13" s="72">
         <f>H25-SUM(H6:H12)</f>
         <v>11276</v>
       </c>
@@ -6510,7 +6516,7 @@
         <f t="shared" ref="I13" si="0">I25-SUM(I6:I12)</f>
         <v>7.2552181720000011</v>
       </c>
-      <c r="J13" s="76" t="s">
+      <c r="J13" s="75" t="s">
         <v>35</v>
       </c>
       <c r="K13" s="33">
@@ -6530,16 +6536,16 @@
       <c r="D14" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="70">
+      <c r="E14" s="69">
         <v>0</v>
       </c>
       <c r="F14" s="58">
         <v>104865</v>
       </c>
-      <c r="G14" s="70">
+      <c r="G14" s="69">
         <v>241612</v>
       </c>
-      <c r="H14" s="70">
+      <c r="H14" s="69">
         <v>0</v>
       </c>
       <c r="I14" s="64">
@@ -6565,16 +6571,16 @@
       <c r="D15" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="71">
+      <c r="E15" s="70">
         <v>585823</v>
       </c>
       <c r="F15" s="59">
         <v>370816</v>
       </c>
-      <c r="G15" s="71">
+      <c r="G15" s="70">
         <v>1156347</v>
       </c>
-      <c r="H15" s="71">
+      <c r="H15" s="70">
         <v>292281</v>
       </c>
       <c r="I15" s="65">
@@ -6600,20 +6606,20 @@
       <c r="D16" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="71">
+      <c r="E16" s="70">
         <v>565505</v>
       </c>
       <c r="F16" s="59">
         <v>419206</v>
       </c>
-      <c r="G16" s="71">
+      <c r="G16" s="70">
         <v>1388642</v>
       </c>
-      <c r="H16" s="71">
+      <c r="H16" s="70">
         <v>820769</v>
       </c>
       <c r="I16" s="65">
-        <v>13.255516849999999</v>
+        <v>13.15709</v>
       </c>
       <c r="J16" s="27">
         <v>6.6060960288331231E-3</v>
@@ -6635,19 +6641,19 @@
       <c r="D17" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="72">
+      <c r="E17" s="71">
         <v>0</v>
       </c>
       <c r="F17" s="60">
         <v>0</v>
       </c>
-      <c r="G17" s="72">
+      <c r="G17" s="71">
         <v>182479</v>
       </c>
-      <c r="H17" s="72">
+      <c r="H17" s="71">
         <v>0</v>
       </c>
-      <c r="I17" s="66">
+      <c r="I17" s="82">
         <f>958895155/1000000000</f>
         <v>0.958895155</v>
       </c>
@@ -6665,28 +6671,28 @@
       <c r="B18" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="68" t="s">
+      <c r="C18" s="67" t="s">
         <v>63</v>
       </c>
       <c r="D18" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="72">
+      <c r="E18" s="71">
         <v>213146</v>
       </c>
       <c r="F18" s="60">
         <v>134511</v>
       </c>
-      <c r="G18" s="72">
+      <c r="G18" s="71">
         <v>395601</v>
       </c>
-      <c r="H18" s="72">
+      <c r="H18" s="71">
         <v>0</v>
       </c>
       <c r="I18" s="65">
         <v>14.351532068999999</v>
       </c>
-      <c r="J18" s="83" t="s">
+      <c r="J18" s="80" t="s">
         <v>44</v>
       </c>
       <c r="K18" s="28">
@@ -6706,20 +6712,20 @@
       <c r="D19" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="71">
+      <c r="E19" s="70">
         <v>607775</v>
       </c>
       <c r="F19" s="59">
         <v>711376</v>
       </c>
-      <c r="G19" s="71">
+      <c r="G19" s="70">
         <v>4809608</v>
       </c>
-      <c r="H19" s="71">
+      <c r="H19" s="70">
         <v>0</v>
       </c>
       <c r="I19" s="65">
-        <v>47.697872713999999</v>
+        <v>47.61772002</v>
       </c>
       <c r="J19" s="27">
         <v>3.0596432575689708E-2</v>
@@ -6741,16 +6747,16 @@
       <c r="D20" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="71">
+      <c r="E20" s="70">
         <v>2</v>
       </c>
       <c r="F20" s="59">
         <v>38652</v>
       </c>
-      <c r="G20" s="71">
+      <c r="G20" s="70">
         <v>424695</v>
       </c>
-      <c r="H20" s="71">
+      <c r="H20" s="70">
         <v>0</v>
       </c>
       <c r="I20" s="65">
@@ -6776,7 +6782,7 @@
       <c r="D21" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="74">
+      <c r="E21" s="73">
         <f>E26-SUM(E14:E20)</f>
         <v>55131</v>
       </c>
@@ -6784,17 +6790,17 @@
         <f t="shared" ref="F21" si="1">F26-SUM(F14:F20)</f>
         <v>63881</v>
       </c>
-      <c r="G21" s="74">
+      <c r="G21" s="73">
         <f>G26-SUM(G14:G20)</f>
         <v>270974</v>
       </c>
-      <c r="H21" s="74">
+      <c r="H21" s="73">
         <f>H26-SUM(H14:H20)</f>
         <v>3988</v>
       </c>
-      <c r="I21" s="63">
+      <c r="I21" s="85">
         <f>I26-SUM(I14:I20)</f>
-        <v>44.234137726000014</v>
+        <v>44.450464835000005</v>
       </c>
       <c r="J21" s="32" t="s">
         <v>35</v>
@@ -6828,7 +6834,7 @@
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
       <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
+      <c r="J23" s="81"/>
       <c r="K23" s="4"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -6839,21 +6845,21 @@
       <c r="D24" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="77">
+      <c r="E24" s="76">
         <v>2347516</v>
       </c>
-      <c r="F24" s="77">
+      <c r="F24" s="76">
         <v>2089192</v>
       </c>
-      <c r="G24" s="77">
+      <c r="G24" s="76">
         <v>9676953</v>
       </c>
-      <c r="H24" s="77">
+      <c r="H24" s="76">
         <v>6615664</v>
       </c>
       <c r="I24" s="18">
         <f>SUM(I25:I26)</f>
-        <v>162.44523911500002</v>
+        <v>162.48298668000001</v>
       </c>
       <c r="J24" s="6"/>
       <c r="K24" s="10">
@@ -6868,19 +6874,19 @@
       <c r="D25" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="69">
+      <c r="E25" s="68">
         <v>320134</v>
       </c>
-      <c r="F25" s="69">
+      <c r="F25" s="68">
         <v>245885</v>
       </c>
-      <c r="G25" s="69">
+      <c r="G25" s="68">
         <v>806995</v>
       </c>
-      <c r="H25" s="69">
+      <c r="H25" s="68">
         <v>5498626</v>
       </c>
-      <c r="I25" s="78">
+      <c r="I25" s="13">
         <v>18.705668322000001</v>
       </c>
       <c r="J25" s="3"/>
@@ -6896,30 +6902,39 @@
       <c r="D26" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E26" s="79">
+      <c r="E26" s="77">
         <v>2027382</v>
       </c>
-      <c r="F26" s="79">
+      <c r="F26" s="77">
         <v>1843307</v>
       </c>
-      <c r="G26" s="79">
+      <c r="G26" s="77">
         <v>8869958</v>
       </c>
-      <c r="H26" s="79">
+      <c r="H26" s="77">
         <v>1117038</v>
       </c>
-      <c r="I26" s="80">
-        <v>143.73957079300001</v>
+      <c r="I26" s="86">
+        <v>143.777318358</v>
       </c>
       <c r="J26" s="7"/>
       <c r="K26" s="14">
         <v>2015</v>
       </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I28" s="83"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I29" s="83"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I31" s="84"/>
     </row>
     <row r="38" ht="14.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="63" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="27" max="16383" man="1"/>
   </rowBreaks>
@@ -6931,7 +6946,7 @@
   <dimension ref="A2:A30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6986,7 +7001,7 @@
     </row>
     <row r="11" spans="1:1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="41" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="27" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>